<commit_message>
Update Performance, Testaus, Toteutus
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -120,10 +120,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Taulukko1!$A$2:$A$10</c:f>
+              <c:f>Taulukko1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5.0</c:v>
                 </c:pt>
@@ -131,24 +131,30 @@
                   <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>15.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>20.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>25.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>30.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>40.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>60.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>80.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -156,10 +162,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Taulukko1!$B$2:$B$10</c:f>
+              <c:f>Taulukko1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.001</c:v>
                 </c:pt>
@@ -167,24 +173,30 @@
                   <c:v>0.002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.002</c:v>
+                  <c:v>0.003</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.005</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.006</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.009</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>0.015</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.027</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>0.078</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>0.189</c:v>
                 </c:pt>
               </c:numCache>
@@ -212,10 +224,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Taulukko1!$A$2:$A$10</c:f>
+              <c:f>Taulukko1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5.0</c:v>
                 </c:pt>
@@ -223,24 +235,30 @@
                   <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>15.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>20.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>25.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>30.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>40.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>60.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>80.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -248,10 +266,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Taulukko1!$C$2:$C$10</c:f>
+              <c:f>Taulukko1!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -259,9 +277,15 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.01</c:v>
+                  <c:v>0.001</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.117</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.409</c:v>
                 </c:pt>
               </c:numCache>
@@ -277,11 +301,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121620552"/>
-        <c:axId val="2122105112"/>
+        <c:axId val="-2144084616"/>
+        <c:axId val="-2144095224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121620552"/>
+        <c:axId val="-2144084616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80.0"/>
@@ -333,15 +357,16 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2122105112"/>
+        <c:crossAx val="-2144095224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122105112"/>
+        <c:axId val="-2144095224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -379,7 +404,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121620552"/>
+        <c:crossAx val="-2144084616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -433,7 +458,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -778,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -824,69 +849,90 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>6.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C5">
-        <v>0.40899999999999997</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>8.9999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.11700000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>1.4999999999999999E-2</v>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C7">
+        <v>0.40899999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B8">
-        <v>2.7E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>7.8E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
         <v>80</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>0.189</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>